<commit_message>
Updating the login api testcases with testdata
</commit_message>
<xml_diff>
--- a/src/test/resources/API_Users.xlsx
+++ b/src/test/resources/API_Users.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="7500"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="UserRegister" sheetId="1" r:id="rId1"/>
+    <sheet name="Login" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Testcases</t>
   </si>
@@ -108,6 +109,21 @@
   </si>
   <si>
     <t>Password must be between 6 and 30 characters</t>
+  </si>
+  <si>
+    <t>Expected Message</t>
+  </si>
+  <si>
+    <t>Login successful</t>
+  </si>
+  <si>
+    <t>test0067.com</t>
+  </si>
+  <si>
+    <t>Invalid password</t>
+  </si>
+  <si>
+    <t>tEST</t>
   </si>
 </sst>
 </file>
@@ -138,7 +154,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFF46E1E"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -591,26 +607,26 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -734,10 +750,14 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1079,11 +1099,11 @@
   <sheetPr/>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="4" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="4" outlineLevelCol="6"/>
   <cols>
     <col min="1" max="1" width="18.1416666666667" customWidth="1"/>
     <col min="3" max="3" width="24.625" customWidth="1"/>
@@ -1216,4 +1236,113 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.8" outlineLevelRow="3" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="16.6" customWidth="1"/>
+    <col min="2" max="2" width="20.6" customWidth="1"/>
+    <col min="3" max="3" width="14.4" customWidth="1"/>
+    <col min="5" max="5" width="8.8" style="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="b">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3">
+        <v>200</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="6">
+        <v>400</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="6">
+        <v>400</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="test004@admin.com" tooltip="mailto:test004@admin.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="test@1234"/>
+    <hyperlink ref="B4" r:id="rId1" display="test004@admin.com"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding thr excel utils changes
</commit_message>
<xml_diff>
--- a/src/test/resources/API_Users.xlsx
+++ b/src/test/resources/API_Users.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
   <si>
     <t>Testcases</t>
   </si>
@@ -120,10 +120,16 @@
     <t>test0067.com</t>
   </si>
   <si>
-    <t>Invalid password</t>
-  </si>
-  <si>
     <t>tEST</t>
+  </si>
+  <si>
+    <t>Incorrect Password</t>
+  </si>
+  <si>
+    <t>test@12345678</t>
+  </si>
+  <si>
+    <t>Incorrect email address or password</t>
   </si>
 </sst>
 </file>
@@ -136,7 +142,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,6 +169,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -623,134 +637,134 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -758,6 +772,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1241,13 +1256,13 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.8" outlineLevelRow="3" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.8" outlineLevelRow="4" outlineLevelCol="5"/>
   <cols>
     <col min="1" max="1" width="16.6" customWidth="1"/>
     <col min="2" max="2" width="20.6" customWidth="1"/>
@@ -1318,13 +1333,13 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>30</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1334,6 +1349,26 @@
       </c>
       <c r="F4" s="4" t="s">
         <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="6">
+        <v>400</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1341,6 +1376,8 @@
     <hyperlink ref="B2" r:id="rId1" display="test004@admin.com" tooltip="mailto:test004@admin.com"/>
     <hyperlink ref="C3" r:id="rId2" display="test@1234"/>
     <hyperlink ref="B4" r:id="rId1" display="test004@admin.com"/>
+    <hyperlink ref="B5" r:id="rId1" display="test004@admin.com" tooltip="mailto:test004@admin.com"/>
+    <hyperlink ref="C5" r:id="rId3" display="test@12345678" tooltip="mailto:test@12345678"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
testdata for change password
</commit_message>
<xml_diff>
--- a/src/test/resources/API_Users.xlsx
+++ b/src/test/resources/API_Users.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9000" activeTab="1"/>
+    <workbookView windowWidth="23040" windowHeight="9000" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="UserRegister" sheetId="1" r:id="rId1"/>
     <sheet name="Login" sheetId="2" r:id="rId2"/>
+    <sheet name="ChangePassword" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="48">
   <si>
     <t>Testcases</t>
   </si>
@@ -48,7 +49,7 @@
     <t>status</t>
   </si>
   <si>
-    <t>expectedMessage</t>
+    <t>Expected Message</t>
   </si>
   <si>
     <t>Success</t>
@@ -111,9 +112,6 @@
     <t>Password must be between 6 and 30 characters</t>
   </si>
   <si>
-    <t>Expected Message</t>
-  </si>
-  <si>
     <t>Login successful</t>
   </si>
   <si>
@@ -130,6 +128,51 @@
   </si>
   <si>
     <t>Incorrect email address or password</t>
+  </si>
+  <si>
+    <t>current password</t>
+  </si>
+  <si>
+    <t>new password</t>
+  </si>
+  <si>
+    <t>test@12345</t>
+  </si>
+  <si>
+    <t>test@76897</t>
+  </si>
+  <si>
+    <t>The password was successfully updated</t>
+  </si>
+  <si>
+    <t>Invalid Current Password</t>
+  </si>
+  <si>
+    <t>Current password must be between 6 and 30 characters</t>
+  </si>
+  <si>
+    <t>Incorrect Current Password</t>
+  </si>
+  <si>
+    <t>test@673456789</t>
+  </si>
+  <si>
+    <t>test@45678</t>
+  </si>
+  <si>
+    <t>The current password is incorrect</t>
+  </si>
+  <si>
+    <t>Invalid New Password</t>
+  </si>
+  <si>
+    <t>New password must be between 6 and 30 characters</t>
+  </si>
+  <si>
+    <t>New Password Same As Current Password</t>
+  </si>
+  <si>
+    <t>The new password should be different from the current password</t>
   </si>
 </sst>
 </file>
@@ -151,32 +194,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFF46E1E"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF0072C5"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFF46E1E"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
       <name val="Aptos Narrow"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -636,7 +679,7 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -766,13 +809,13 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="6" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1115,7 +1158,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.8" outlineLevelRow="4" outlineLevelCol="6"/>
@@ -1123,12 +1166,12 @@
     <col min="1" max="1" width="18.1416666666667" customWidth="1"/>
     <col min="3" max="3" width="24.625" customWidth="1"/>
     <col min="4" max="4" width="19.8583333333333" customWidth="1"/>
-    <col min="6" max="6" width="11.425" style="1" customWidth="1"/>
+    <col min="6" max="6" width="11.425" style="4" customWidth="1"/>
     <col min="7" max="7" width="37.5666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1143,7 +1186,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -1166,7 +1209,7 @@
       <c r="E2" t="b">
         <v>1</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G2" t="s">
@@ -1189,7 +1232,7 @@
       <c r="E3" t="b">
         <v>0</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="4" t="s">
         <v>15</v>
       </c>
       <c r="G3" t="s">
@@ -1212,7 +1255,7 @@
       <c r="E4" t="b">
         <v>0</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G4" t="s">
@@ -1235,7 +1278,7 @@
       <c r="E5" t="b">
         <v>0</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="F5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="G5" t="s">
@@ -1258,8 +1301,8 @@
   <sheetPr/>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.8" outlineLevelRow="4" outlineLevelCol="5"/>
@@ -1267,12 +1310,12 @@
     <col min="1" max="1" width="16.6" customWidth="1"/>
     <col min="2" max="2" width="20.6" customWidth="1"/>
     <col min="3" max="3" width="14.4" customWidth="1"/>
-    <col min="5" max="5" width="8.8" style="1"/>
+    <col min="5" max="5" width="8.8" style="4"/>
     <col min="6" max="6" width="17.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1282,13 +1325,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="F1" t="s">
-        <v>27</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1304,11 +1347,11 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2" s="6">
         <v>200</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>28</v>
+      <c r="F2" s="3" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1316,18 +1359,18 @@
         <v>17</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="7">
         <v>400</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1335,40 +1378,40 @@
       <c r="A4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="7">
         <v>400</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="7" t="s">
-        <v>32</v>
+      <c r="C5" s="1" t="s">
+        <v>31</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="7">
         <v>400</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>33</v>
+      <c r="F5" s="3" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1382,4 +1425,182 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="13.8" outlineLevelRow="5" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="37.1" customWidth="1"/>
+    <col min="2" max="2" width="23.7" customWidth="1"/>
+    <col min="3" max="3" width="19.5" customWidth="1"/>
+    <col min="4" max="5" width="12.1" customWidth="1"/>
+    <col min="7" max="7" width="24.1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>200</v>
+      </c>
+      <c r="G2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>400</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" t="b">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>400</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" t="b">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>400</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>400</v>
+      </c>
+      <c r="G6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" display="test@12345"/>
+    <hyperlink ref="D2" r:id="rId2" display="test@76897"/>
+    <hyperlink ref="C3" r:id="rId3" display="test"/>
+    <hyperlink ref="D3" r:id="rId2" display="test@76897"/>
+    <hyperlink ref="B2" r:id="rId4" display="test004@admin.com"/>
+    <hyperlink ref="B3" r:id="rId4" display="test004@admin.com"/>
+    <hyperlink ref="B4" r:id="rId4" display="test004@admin.com"/>
+    <hyperlink ref="C4" r:id="rId5" display="test@673456789"/>
+    <hyperlink ref="D4" r:id="rId6" display="test@45678"/>
+    <hyperlink ref="B5" r:id="rId4" display="test004@admin.com"/>
+    <hyperlink ref="C5" r:id="rId1" display="test@12345"/>
+    <hyperlink ref="B6" r:id="rId4" display="test004@admin.com"/>
+    <hyperlink ref="C6" r:id="rId1" display="test@12345"/>
+    <hyperlink ref="D6" r:id="rId1" display="test@12345"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>